<commit_message>
Fixed CCDI queries and ICDC index issue
</commit_message>
<xml_diff>
--- a/InputFiles/CCDI/TC01_CCDI_phs002371_Sex-Male.xlsx
+++ b/InputFiles/CCDI/TC01_CCDI_phs002371_Sex-Male.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tatekaraa\Automation\08-20-24\Commons_Automation\InputFiles\CCDI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sohilz2/Automation/poc-09-25-2024/Commons_Automation/InputFiles/CCDI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CE97157-050F-4735-9CDF-4D5B2188C2B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27E6F696-277A-B144-BAB9-CDE172F2B977}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21480" yWindow="-1875" windowWidth="21840" windowHeight="13140" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="30240" yWindow="-1880" windowWidth="21840" windowHeight="13140" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -69,32 +69,6 @@
   </si>
   <si>
     <t>SELECT
-    p.participant_id AS "Participant ID",
-    st.study_id AS "Study ID",
-    COALESCE(p.sex_at_birth, '') AS "Sex",
-    COALESCE(p.race, '') AS "Race",
-    COALESCE(p.ethnicity, '') AS "Ethnicity",
-    COALESCE(CAST(p.alternate_participant_id AS INT), '') AS "Alternate ID"
-FROM 
-    df_participant p
-JOIN 
-    df_study st ON p."study.id" = st.id
-LEFT JOIN 
-    df_sample smp ON smp."participant.id" = p.participant_id
-LEFT JOIN 
-    df_diagnosis diag ON diag."participant.id" = p.participant_id
-LEFT JOIN 
-    df_publication pub ON pub."study.id" = st.study_id
-LEFT JOIN 
-    df_sequencing_file sqf ON sqf."sample.id" = smp.sample_id
-WHERE 
-    st.study_id = 'phs002371' AND p.sex_at_birth = 'Male'
-ORDER BY 
-    p.participant_id ASC
-LIMIT 100;</t>
-  </si>
-  <si>
-    <t>SELECT
     COUNT(DISTINCT st.study_id) AS "Studies",
     COUNT(DISTINCT p.participant_id) AS "Participants",
     COUNT(DISTINCT smp.sample_id) AS "Samples",
@@ -254,14 +228,46 @@
     sqf.file_name ASC
 LIMIT 100;</t>
   </si>
+  <si>
+    <t>SELECT
+    p.participant_id AS "Participant ID",
+    st.study_id AS "Study ID",
+    COALESCE(p.sex_at_birth, '') AS "Sex",
+    COALESCE(p.race, '') AS "Race",
+    COALESCE(CAST(p.alternate_participant_id AS INT), '') AS "Synonym Participant ID"
+FROM 
+    df_participant p
+JOIN 
+    df_study st ON p."study.id" = st.id
+LEFT JOIN 
+    df_sample smp ON smp."participant.id" = p.participant_id
+LEFT JOIN 
+    df_diagnosis diag ON diag."participant.id" = p.participant_id
+LEFT JOIN 
+    df_publication pub ON pub."study.id" = st.study_id
+LEFT JOIN 
+    df_sequencing_file sqf ON sqf."sample.id" = smp.sample_id
+WHERE 
+    st.study_id = 'phs002371' AND p.sex_at_birth = 'Male'
+ORDER BY 
+    p.participant_id ASC
+LIMIT 100;</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -335,14 +341,17 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -675,18 +684,18 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="75.85546875" customWidth="1"/>
-    <col min="4" max="4" width="70.140625" customWidth="1"/>
-    <col min="5" max="5" width="63.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="75.83203125" customWidth="1"/>
+    <col min="4" max="4" width="70.1640625" customWidth="1"/>
+    <col min="5" max="5" width="63.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -703,68 +712,68 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="378" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="388" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="D2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>12</v>
       </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
     </row>
-    <row r="3" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3" s="3"/>
     </row>
-    <row r="4" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" s="3"/>
     </row>
-    <row r="5" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" s="2"/>
     </row>
-    <row r="6" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6" s="2"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C8" s="1"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>